<commit_message>
Video analysis: Optical flow
</commit_message>
<xml_diff>
--- a/ComputerVision Basic.xlsx
+++ b/ComputerVision Basic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive - Hanoi University of Science and Technology\Desktop\Learn OpenCV\Learn_OpenCV_Arrow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767AC63A-D149-43FF-BB50-566F2E355202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F82B172-FED8-424C-BD27-B6A51469ABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Estimate (h)</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>17/6/2024</t>
+  </si>
+  <si>
+    <t>25/6/2024</t>
+  </si>
+  <si>
+    <t>18,24/6/2024</t>
   </si>
 </sst>
 </file>
@@ -573,15 +579,15 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="46.90625" customWidth="1"/>
     <col min="4" max="4" width="42.453125" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" style="16"/>
+    <col min="5" max="5" width="15.6328125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -888,7 +894,9 @@
       <c r="D28" s="10">
         <v>3</v>
       </c>
-      <c r="E28" s="15"/>
+      <c r="E28" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15.5">
       <c r="A29" s="18"/>
@@ -908,7 +916,9 @@
       <c r="D30" s="10">
         <v>5</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15.5">
       <c r="A31" s="19"/>

</xml_diff>